<commit_message>
SVM, LR, DNN comparison
</commit_message>
<xml_diff>
--- a/QandAData.xlsx
+++ b/QandAData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
   <si>
     <t xml:space="preserve">Answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
   </si>
   <si>
     <t xml:space="preserve">How to do a Birth Chirp?</t>
@@ -398,7 +401,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -406,11 +409,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="11" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -418,7 +421,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -442,16 +445,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.8785425101215"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="122.117408906883"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="84.1943319838057"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -462,228 +465,318 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="195" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>